<commit_message>
főbb határidők és lépések felvitele - nem teljesen feltöltött
</commit_message>
<xml_diff>
--- a/projekt_mintamenet.xlsx
+++ b/projekt_mintamenet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24923"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corvusoid/Documents/Hengersor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://plkik.sharepoint.com/sites/Esti_projektmunka_gyakorloter/Megosztott dokumentumok/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA96F48-B527-BD47-8201-91C9E582AFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="240" documentId="13_ncr:1_{9AA96F48-B527-BD47-8201-91C9E582AFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32E06B78-92F9-4D81-A592-DF5C719A8FD9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{39ABA147-C24E-9C46-B36D-D7DDC8F00C1D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="52">
   <si>
     <t>Projektmunka terv</t>
   </si>
@@ -58,37 +58,142 @@
     <t>Megjegyzés</t>
   </si>
   <si>
-    <t>Weboldal - munkafolyamatok</t>
-  </si>
-  <si>
-    <t>Fejlesztés</t>
-  </si>
-  <si>
-    <t>2022.22.25</t>
-  </si>
-  <si>
-    <t>Megbeszélés</t>
-  </si>
-  <si>
-    <t>Kész</t>
-  </si>
-  <si>
-    <t>Képek szerkesztése</t>
-  </si>
-  <si>
-    <t>Gombok elkészítése</t>
-  </si>
-  <si>
-    <t>Tervezés</t>
-  </si>
-  <si>
-    <t>Adatbázis - munkafolyamatok</t>
-  </si>
-  <si>
-    <t>Tesztelés</t>
-  </si>
-  <si>
-    <t>Hibás</t>
+    <t>weboldal</t>
+  </si>
+  <si>
+    <t>Ádám</t>
+  </si>
+  <si>
+    <t>drótváz</t>
+  </si>
+  <si>
+    <t>Develop</t>
+  </si>
+  <si>
+    <t>egyed-kapcsolat diagram</t>
+  </si>
+  <si>
+    <t>Melinda</t>
+  </si>
+  <si>
+    <t>esetdiagram</t>
+  </si>
+  <si>
+    <t>0. Kezdőoldal - introval</t>
+  </si>
+  <si>
+    <t>Melinda / Ádám</t>
+  </si>
+  <si>
+    <t xml:space="preserve">felület elkészítése </t>
+  </si>
+  <si>
+    <t>bemutatkozó szöveg</t>
+  </si>
+  <si>
+    <t>intro/intro átugrás</t>
+  </si>
+  <si>
+    <t>opcionális hogy lesz</t>
+  </si>
+  <si>
+    <t>1. Menüoldal</t>
+  </si>
+  <si>
+    <t>design, linkek, gombok</t>
+  </si>
+  <si>
+    <t>képek</t>
+  </si>
+  <si>
+    <t>2. Regisztráció / bejelentkezés</t>
+  </si>
+  <si>
+    <t>regisztrációs felület elkészíteni</t>
+  </si>
+  <si>
+    <t>sikeres regisztrációs felugró ablakok elkészítése (gazdi/menhely)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email küldés kialakítása </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gazdiknak visszaigazolás weblink+usernév
+menhelynek asztali alkalmazás becsatolva
+visszaigazoló emailben adatkezelési tájékoztató, oldathasználati tájékoztató és figyelmeztetés, hogy ha nem lép be x napig akkor töröljük a fiókját
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">profilablak </t>
+  </si>
+  <si>
+    <t>üdvözlés, kijelentkező gomb, mentett keresések lista</t>
+  </si>
+  <si>
+    <t>profilablak létrehozása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mentett keresések megjelenítése / kitörölhetőség </t>
+  </si>
+  <si>
+    <t>3. kutya kereső felület</t>
+  </si>
+  <si>
+    <t>felület kinézetét megtervezni</t>
+  </si>
+  <si>
+    <t>4. adományozás és menhely infók</t>
+  </si>
+  <si>
+    <t>asztali alkalmazás</t>
+  </si>
+  <si>
+    <t>itt lehet a kutyák adatait felvinni</t>
+  </si>
+  <si>
+    <t>adatbázis kapcsolatot kiépíteni</t>
+  </si>
+  <si>
+    <t>installer készítése</t>
+  </si>
+  <si>
+    <t>letrehozni a telepítőt, amit emailben kap meg regisztráció után a menhely</t>
+  </si>
+  <si>
+    <t>adatkarbantartás ellenőrzése</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a menhely itt állítja a felvitt kutyák státuszát, törlés, adatmódosítás, lekérdezés, lehetőleg egy </t>
+  </si>
+  <si>
+    <t>adatbázis</t>
+  </si>
+  <si>
+    <t>kiterjesztett egyed- kapcsolat diagram</t>
+  </si>
+  <si>
+    <t>regisztrált adatok adatbázisba mentése</t>
+  </si>
+  <si>
+    <t>felrögzített kutya adatok adatbázisba mentése</t>
+  </si>
+  <si>
+    <t>kutyák státuszállításait logolni kell</t>
+  </si>
+  <si>
+    <t>ha x napig inaktív egy kutya, akkor egyeztetni kell a menhellyel, hogy kezelje/törölje</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Error</t>
   </si>
 </sst>
 </file>
@@ -96,10 +201,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0&quot; nap&quot;"/>
-    <numFmt numFmtId="165" formatCode="&quot;H-&quot;0000"/>
+    <numFmt numFmtId="164" formatCode="&quot;H-&quot;0000"/>
+    <numFmt numFmtId="165" formatCode="0&quot; day&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,8 +243,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,8 +274,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -320,79 +460,145 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,211 +914,822 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8E7F18-5A48-1C46-BD03-BEEDB5094022}">
-  <dimension ref="B1:H15"/>
+  <dimension ref="B1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="2" max="2" width="38.375" customWidth="1"/>
-    <col min="3" max="4" width="19.875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="19.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="32.375" customWidth="1"/>
+    <col min="1" max="1" width="11" style="11"/>
+    <col min="2" max="2" width="63.375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="11" customWidth="1"/>
+    <col min="6" max="6" width="19.875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="24.5" style="11" customWidth="1"/>
+    <col min="8" max="8" width="64.875" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="11" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="23" customFormat="1" ht="32.1" thickBot="1">
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="2:8" s="4" customFormat="1" ht="31.5">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:8" s="1" customFormat="1" ht="18.95">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:8" s="32" customFormat="1" ht="23.25">
+      <c r="B2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="27">
+        <v>44591</v>
+      </c>
+      <c r="E2" s="28">
+        <f>F2-D2</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="29">
+        <v>44592</v>
+      </c>
+      <c r="G2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5">
-        <v>44590</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="2:8" ht="18.75">
+      <c r="B3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E3" s="7">
+        <f t="shared" ref="E3:E37" si="0">F3-D3</f>
+        <v>7</v>
+      </c>
+      <c r="F3" s="8">
+        <v>44598</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="2:8" ht="18.75">
+      <c r="B4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>44592</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="2:8" ht="18.75">
+      <c r="B5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="8">
+        <v>44592</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="2:8" s="32" customFormat="1" ht="18.75">
+      <c r="B6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="27">
+        <v>44591</v>
+      </c>
+      <c r="E6" s="28">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F6" s="29">
+        <v>44620</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="2:8" ht="18.75">
+      <c r="B7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="8">
+        <v>44592</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="2:8" ht="18.75">
+      <c r="B8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F8" s="8">
+        <v>44598</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="2:8" ht="18.75">
+      <c r="B9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F9" s="8">
+        <v>44598</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" s="32" customFormat="1" ht="18.75">
+      <c r="B10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="27">
+        <v>44591</v>
+      </c>
+      <c r="E10" s="28">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F10" s="29">
+        <v>44620</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="31"/>
+    </row>
+    <row r="11" spans="2:8" s="32" customFormat="1" ht="18.75">
+      <c r="B11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F11" s="8">
+        <v>44620</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="31"/>
+    </row>
+    <row r="12" spans="2:8" ht="18.75">
+      <c r="B12" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F12" s="8">
+        <v>44598</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="2:8" ht="18.75">
+      <c r="B13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F13" s="8">
+        <v>44620</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="2:8" s="32" customFormat="1" ht="18.75">
+      <c r="B14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="27">
+        <v>44591</v>
+      </c>
+      <c r="E14" s="28">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="F14" s="29">
+        <v>44635</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="31"/>
+    </row>
+    <row r="15" spans="2:8" ht="18.75">
+      <c r="B15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="F15" s="8">
+        <v>44635</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="2:8" ht="18.75">
+      <c r="B16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="F16" s="8">
+        <v>44635</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="2:8" ht="91.5" customHeight="1">
+      <c r="B17" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="F17" s="8">
+        <v>44635</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" s="32" customFormat="1" ht="18.75">
+      <c r="B18" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="27">
+        <v>44591</v>
+      </c>
+      <c r="E18" s="28">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F18" s="29">
+        <v>44620</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" s="32" customFormat="1" ht="18.75">
+      <c r="B19" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="31"/>
+    </row>
+    <row r="20" spans="2:8" ht="18.75">
+      <c r="B20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="2:8" s="32" customFormat="1" ht="18.75">
+      <c r="B21" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="27">
+        <v>44591</v>
+      </c>
+      <c r="E21" s="28">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F21" s="29">
+        <v>44620</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="31"/>
+    </row>
+    <row r="22" spans="2:8" ht="18.75">
+      <c r="B22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="2:8" ht="18.75">
+      <c r="B23" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="2:8" s="32" customFormat="1" ht="18.75">
+      <c r="B24" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="27">
+        <v>44591</v>
+      </c>
+      <c r="E24" s="28">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F24" s="33"/>
+      <c r="G24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="31"/>
+    </row>
+    <row r="25" spans="2:8" s="32" customFormat="1" ht="23.25">
+      <c r="B25" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="2:8" ht="18.95">
-      <c r="B3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="10">
-        <v>44590</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2</v>
-      </c>
-      <c r="F3" s="10">
-        <v>44600</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="2:8" ht="18.95">
-      <c r="B4" s="17" t="s">
+      <c r="C25" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="27">
+        <v>44591</v>
+      </c>
+      <c r="E25" s="28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F25" s="29">
+        <v>44592</v>
+      </c>
+      <c r="G25" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="31"/>
+    </row>
+    <row r="26" spans="2:8" ht="18.75">
+      <c r="B26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E26" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="G26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="18.75">
+      <c r="B27" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E27" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="G27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="2:8" ht="18.75">
+      <c r="B28" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E28" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="G28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" spans="2:8" ht="37.5">
+      <c r="B29" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E29" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F29" s="14"/>
+      <c r="G29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="37.5">
+      <c r="B30" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E30" s="7">
+        <f>F30-D30</f>
+        <v>-44591</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="23.25">
+      <c r="B31" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E31" s="7">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F31" s="6">
+        <v>44620</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="18">
-        <v>44591</v>
-      </c>
-      <c r="E4" s="6">
-        <v>5</v>
-      </c>
-      <c r="F4" s="18">
-        <v>44597</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="2:8" ht="18.95">
-      <c r="B5" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="18">
-        <v>44607</v>
-      </c>
-      <c r="E5" s="6">
-        <v>15</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="2:8" ht="18.95">
-      <c r="B6" s="17"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="2:8" ht="18.95">
-      <c r="B7" s="17"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="2:8" ht="18.95">
-      <c r="B8" s="17"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="2:8" ht="18.95">
-      <c r="B9" s="17"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="2:8" ht="18.95">
-      <c r="B10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="2:8" ht="18.95">
-      <c r="B11" s="17"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="2:8" ht="18.95">
-      <c r="B12" s="17"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="2:8" ht="18.95">
-      <c r="B13" s="17"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="2:8" ht="18.95">
-      <c r="B14" s="17"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="2:8" ht="20.100000000000001" thickBot="1">
-      <c r="B15" s="19"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
-    </row>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="2:8" ht="18.75">
+      <c r="B32" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E32" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F32" s="8">
+        <v>44592</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="2:8" ht="18.75">
+      <c r="B33" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E33" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34" spans="2:8" ht="18.75">
+      <c r="B34" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E34" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="18"/>
+    </row>
+    <row r="35" spans="2:8" ht="18.75">
+      <c r="B35" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E35" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="2:8" ht="37.5">
+      <c r="B36" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E36" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="18.75">
+      <c r="B37" s="19"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="6">
+        <v>44591</v>
+      </c>
+      <c r="E37" s="7">
+        <f t="shared" si="0"/>
+        <v>-44591</v>
+      </c>
+      <c r="F37" s="20"/>
+      <c r="G37" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="21"/>
+    </row>
+    <row r="38" spans="2:8" ht="15.75"/>
+    <row r="39" spans="2:8" ht="15.75"/>
+    <row r="40" spans="2:8" ht="15.75"/>
+    <row r="41" spans="2:8" ht="15.75"/>
+    <row r="42" spans="2:8" ht="15.75">
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+    </row>
+    <row r="46" spans="2:8" ht="15.75"/>
+    <row r="47" spans="2:8" ht="15.75"/>
+    <row r="48" spans="2:8" ht="15.75"/>
+    <row r="49" ht="15.75"/>
+    <row r="50" ht="15.75"/>
+    <row r="51" ht="15.75"/>
+    <row r="52" ht="15.75"/>
+    <row r="53" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -923,7 +1740,7 @@
           <x14:formula1>
             <xm:f>'Háttér adatok'!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C15</xm:sqref>
+          <xm:sqref>C2:C37</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -936,7 +1753,7 @@
   <dimension ref="C1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -951,27 +1768,27 @@
     </row>
     <row r="3" spans="3:3">
       <c r="C3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="3:3">
       <c r="C4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1112,12 +1929,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1126,14 +1937,20 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99A92CFD-B1FA-4FCA-AF50-DC9E9DC51401}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96FCF378-3613-4098-AEC9-03B7F93F285D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1DEA722-1A89-4570-ACBD-2A7F40E42575}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1DEA722-1A89-4570-ACBD-2A7F40E42575}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96FCF378-3613-4098-AEC9-03B7F93F285D}"/>
 </file>
</xml_diff>